<commit_message>
read file with js
</commit_message>
<xml_diff>
--- a/black_list.xlsx
+++ b/black_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,6 +552,48 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>203.107.1.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>203.107.1.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>203.107.1.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>203.107.1.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>203.107.1.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>203.107.1.34</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chinh sua checkip neu khong check ra df_malicious hoac df_normal
</commit_message>
<xml_diff>
--- a/black_list.xlsx
+++ b/black_list.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,49 +443,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1.1.1.1</t>
+          <t>112.126.94.107</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>203.107.1.34</t>
+          <t>123.56.228.49</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>203.107.1.33</t>
+          <t>139.99.236.139</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>203.107.1.34</t>
+          <t>158.51.124.38</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>203.107.1.33</t>
+          <t>158.51.124.56</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>203.107.1.34</t>
+          <t>158.51.126.135</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>203.107.1.33</t>
+          <t>185.215.113.66</t>
         </is>
       </c>
     </row>
@@ -499,98 +499,56 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>203.107.1.33</t>
+          <t>217.8.117.10</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>203.107.1.34</t>
+          <t>5.188.226.52</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>203.107.1.33</t>
+          <t>66.187.4.127</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>v20.events.data.microsoft.com</t>
+          <t>66.187.4.169</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>203.107.1.34</t>
+          <t>66.187.4.92</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>203.107.1.33</t>
+          <t>66.187.6.203</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>203.107.1.34</t>
+          <t>92.63.197.112</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>203.107.1.33</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>203.107.1.34</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>203.107.1.34</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>203.107.1.34</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>203.107.1.34</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>203.107.1.34</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>203.107.1.34</t>
+          <t>92.63.197.60</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
hoan thien tinh nang update ioc
</commit_message>
<xml_diff>
--- a/black_list.xlsx
+++ b/black_list.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>